<commit_message>
merge database Quan Ly Nhan Su into ISO
</commit_message>
<xml_diff>
--- a/ISO/db/mergeCodeQLNS.xlsx
+++ b/ISO/db/mergeCodeQLNS.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4506"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="45" windowWidth="20115" windowHeight="7995"/>
+    <workbookView xWindow="240" yWindow="45" windowWidth="19440" windowHeight="7995"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="27">
   <si>
     <t>Stt</t>
   </si>
@@ -137,6 +137,21 @@
   <si>
     <t>changeDMYtoMDY()</t>
   </si>
+  <si>
+    <t>getKhoaByMaBoPhan()</t>
+  </si>
+  <si>
+    <t>DAO</t>
+  </si>
+  <si>
+    <t>ThanhVienDAO</t>
+  </si>
+  <si>
+    <t>UpdateVaiTroTV()</t>
+  </si>
+  <si>
+    <t>KhoaDAO</t>
+  </si>
 </sst>
 </file>
 
@@ -146,7 +161,7 @@
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Arial"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <charset val="163"/>
       <scheme val="minor"/>
@@ -474,20 +489,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="C2:G9"/>
+  <dimension ref="C2:G11"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C7" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="C4" workbookViewId="0">
       <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="5.375" customWidth="1"/>
-    <col min="3" max="3" width="15.25" customWidth="1"/>
-    <col min="4" max="4" width="28.375" customWidth="1"/>
-    <col min="5" max="5" width="32.25" customWidth="1"/>
-    <col min="6" max="6" width="61.875" customWidth="1"/>
-    <col min="7" max="7" width="12.5" style="1" customWidth="1"/>
+    <col min="1" max="1" width="5.42578125" customWidth="1"/>
+    <col min="3" max="3" width="15.28515625" customWidth="1"/>
+    <col min="4" max="4" width="28.42578125" customWidth="1"/>
+    <col min="5" max="5" width="32.28515625" customWidth="1"/>
+    <col min="6" max="6" width="61.85546875" customWidth="1"/>
+    <col min="7" max="7" width="12.42578125" style="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="3:7">
@@ -538,7 +553,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="5" spans="3:7" ht="128.25">
+    <row r="5" spans="3:7" ht="135">
       <c r="C5" s="1">
         <v>3</v>
       </c>
@@ -552,7 +567,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="6" spans="3:7" ht="57">
+    <row r="6" spans="3:7" ht="60">
       <c r="C6" s="1">
         <v>4</v>
       </c>
@@ -569,7 +584,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="7" spans="3:7" ht="114">
+    <row r="7" spans="3:7" ht="120">
       <c r="C7" s="1">
         <v>5</v>
       </c>
@@ -586,7 +601,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="8" spans="3:7" ht="128.25">
+    <row r="8" spans="3:7" ht="135">
       <c r="C8" s="1">
         <v>6</v>
       </c>
@@ -614,6 +629,40 @@
         <v>21</v>
       </c>
       <c r="G9" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="10" spans="3:7">
+      <c r="C10" s="1">
+        <v>8</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="E10" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="F10" t="s">
+        <v>22</v>
+      </c>
+      <c r="G10" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="11" spans="3:7">
+      <c r="C11" s="1">
+        <v>9</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="E11" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="F11" t="s">
+        <v>25</v>
+      </c>
+      <c r="G11" s="1" t="s">
         <v>13</v>
       </c>
     </row>
@@ -628,7 +677,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -640,7 +689,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>